<commit_message>
Switch to Google Sheet for materials & costs
</commit_message>
<xml_diff>
--- a/Course Materials and Costs.xlsx
+++ b/Course Materials and Costs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/janke/Dropbox/satchel/projects/so-you-wanna-code/so-you-wanna-code/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41B4B795-06E4-EC4F-96BD-D2595B8DEB70}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2356A80-8BBE-BE4F-9D84-7C674DC23E65}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="180" yWindow="3820" windowWidth="14860" windowHeight="20560" xr2:uid="{FAFBAC99-EDA2-904A-8438-F3B9654B0E00}"/>
   </bookViews>
@@ -538,7 +538,7 @@
   <dimension ref="B2:E45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B41" sqref="B41"/>
+      <selection activeCell="C36" sqref="C36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -783,8 +783,7 @@
       <c r="B27" t="s">
         <v>37</v>
       </c>
-      <c r="C27" s="4"/>
-      <c r="D27" s="4">
+      <c r="C27" s="4">
         <v>200</v>
       </c>
       <c r="E27" t="s">
@@ -879,11 +878,11 @@
       </c>
       <c r="C40" s="4">
         <f>SUM(C4:C38)</f>
-        <v>493</v>
+        <v>693</v>
       </c>
       <c r="D40" s="4">
         <f>SUM(D4:D38)</f>
-        <v>682</v>
+        <v>482</v>
       </c>
     </row>
     <row r="41" spans="2:5" x14ac:dyDescent="0.2">

</xml_diff>